<commit_message>
Add webpage. Fix bug on database. Modify database for new feature "automatic update active host"
</commit_message>
<xml_diff>
--- a/web_server/ThesisTable.xlsx
+++ b/web_server/ThesisTable.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="135" windowWidth="16275" windowHeight="9525"/>
+    <workbookView xWindow="120" yWindow="135" windowWidth="16275" windowHeight="9525" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="sensor_values" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="22">
   <si>
     <t>record_count</t>
   </si>
@@ -73,6 +73,15 @@
   </si>
   <si>
     <t>autoincrement</t>
+  </si>
+  <si>
+    <t>active_state</t>
+  </si>
+  <si>
+    <t>0 for inactive</t>
+  </si>
+  <si>
+    <t>1 for active</t>
   </si>
 </sst>
 </file>
@@ -413,8 +422,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -496,54 +505,58 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="3" max="3" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>12</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>13</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
       <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>15</v>
       </c>
       <c r="E2" t="s">
         <v>15</v>
@@ -551,17 +564,20 @@
       <c r="F2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
       <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
         <v>17</v>
       </c>
-      <c r="C3" t="s">
-        <v>16</v>
-      </c>
       <c r="D3" t="s">
         <v>16</v>
       </c>
@@ -571,10 +587,23 @@
       <c r="F3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>